<commit_message>
new plots and fixed deaths
</commit_message>
<xml_diff>
--- a/RubellaModel.xlsx
+++ b/RubellaModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03B725E-E164-3546-966E-2DCEAC1E1366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D971C39-2D39-AE49-A2E5-FF4DD0558567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="universal" sheetId="1" r:id="rId1"/>
@@ -738,7 +738,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;R&quot;#,##0_);[Red]\(&quot;R&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -758,12 +758,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFDF3079"/>
-      <name val="Monaco"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -841,23 +835,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,28 +1084,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1154,7 +1147,7 @@
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1"/>
       <c r="D5" s="3"/>
       <c r="F5" s="3"/>
@@ -1181,22 +1174,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1287,7 +1280,7 @@
       <c r="B6" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>219</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1327,7 +1320,7 @@
       <c r="B8" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>205</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1347,7 +1340,7 @@
       <c r="B9" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>203</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1367,7 +1360,7 @@
       <c r="B10" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>187</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1387,7 +1380,7 @@
       <c r="B11" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>227</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1467,7 +1460,7 @@
       <c r="B15" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>189</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1507,7 +1500,7 @@
       <c r="B17" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>191</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1547,7 +1540,7 @@
       <c r="B19" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>208</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1576,43 +1569,43 @@
   <dimension ref="A1:L138"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>202</v>
       </c>
     </row>
@@ -1633,7 +1626,7 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <f t="shared" ref="F2:F13" si="0">1-EXP(-0.95*A2)</f>
         <v>0.61325897654549877</v>
       </c>
@@ -1653,6 +1646,9 @@
       <c r="K2">
         <f>J2/120</f>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1672,7 +1668,7 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f t="shared" si="0"/>
         <v>0.85043138077736491</v>
       </c>
@@ -1692,6 +1688,9 @@
       <c r="K3">
         <f t="shared" ref="K3:K66" si="2">J3/120</f>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1711,7 +1710,7 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f t="shared" si="0"/>
         <v>0.94215567912516152</v>
       </c>
@@ -1731,6 +1730,9 @@
       <c r="K4">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1750,7 +1752,7 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>0.97762922814383435</v>
       </c>
@@ -1770,6 +1772,9 @@
       <c r="K5">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1789,7 +1794,7 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>0.99134830479687941</v>
       </c>
@@ -1809,6 +1814,9 @@
       <c r="K6">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1829,7 +1837,7 @@
         <f>0.847*0.97*0.85</f>
         <v>0.6983514999999999</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f t="shared" si="0"/>
         <v>0.99665403454252877</v>
       </c>
@@ -1849,6 +1857,9 @@
       <c r="K7">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1868,7 +1879,7 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f t="shared" si="0"/>
         <v>0.99870597789453419</v>
       </c>
@@ -1888,6 +1899,9 @@
       <c r="K8">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1907,7 +1921,7 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f t="shared" si="0"/>
         <v>0.99949954856655943</v>
       </c>
@@ -1927,6 +1941,9 @@
       <c r="K9">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1946,7 +1963,7 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>0.99980645490044195</v>
       </c>
@@ -1966,6 +1983,9 @@
       <c r="K10">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1985,7 +2005,7 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>0.99992514817011235</v>
       </c>
@@ -2005,6 +2025,9 @@
       <c r="K11">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2024,7 +2047,7 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <f t="shared" si="0"/>
         <v>0.99997105172670175</v>
       </c>
@@ -2044,6 +2067,9 @@
       <c r="K12">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2064,7 +2090,7 @@
         <f>0.72*0.97*0.85</f>
         <v>0.59363999999999995</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <f t="shared" si="0"/>
         <v>0.99998880451515737</v>
       </c>
@@ -2084,6 +2110,9 @@
       <c r="K13">
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2123,6 +2152,9 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
@@ -2161,8 +2193,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2199,9 +2234,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="L16" s="4"/>
+      <c r="L16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2238,8 +2275,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2276,8 +2316,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2314,8 +2357,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2352,8 +2398,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2390,8 +2439,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2428,8 +2480,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2466,8 +2521,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2504,8 +2562,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2542,8 +2603,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2580,8 +2644,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2618,8 +2685,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2656,8 +2726,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2694,8 +2767,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2732,8 +2808,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2770,8 +2849,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2808,8 +2890,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2846,8 +2931,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2884,8 +2972,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2922,8 +3013,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2960,8 +3054,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2998,8 +3095,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3036,8 +3136,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3074,8 +3177,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3112,8 +3218,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3150,8 +3259,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3188,8 +3300,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3226,8 +3341,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3264,8 +3382,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3302,8 +3423,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3340,8 +3464,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
     </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3378,8 +3505,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
     </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3416,8 +3546,11 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3454,15 +3587,18 @@
         <f t="shared" si="2"/>
         <v>8.3333333333333332E-3</v>
       </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>48</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>84</v>
       </c>
       <c r="D50" s="1">
@@ -3479,7 +3615,7 @@
         <f>1/365</f>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H50" s="10" t="s">
+      <c r="H50" s="9" t="s">
         <v>84</v>
       </c>
       <c r="I50">
@@ -3492,8 +3628,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3530,15 +3669,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
     </row>
-    <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="1">
         <v>72</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D52" s="1">
@@ -3555,7 +3697,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="H52" s="9" t="s">
         <v>86</v>
       </c>
       <c r="I52">
@@ -3568,8 +3710,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3606,15 +3751,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="1">
         <v>96</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>88</v>
       </c>
       <c r="D54" s="1">
@@ -3631,7 +3779,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="9" t="s">
         <v>88</v>
       </c>
       <c r="I54">
@@ -3644,8 +3792,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3682,15 +3833,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="1">
         <v>120</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>90</v>
       </c>
       <c r="D56" s="1">
@@ -3707,7 +3861,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="H56" s="9" t="s">
         <v>90</v>
       </c>
       <c r="I56">
@@ -3720,8 +3874,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
     </row>
-    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3758,15 +3915,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>144</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D58" s="1">
@@ -3783,7 +3943,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H58" s="10" t="s">
+      <c r="H58" s="9" t="s">
         <v>92</v>
       </c>
       <c r="I58">
@@ -3796,8 +3956,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
     </row>
-    <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3834,15 +3997,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
     </row>
-    <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1">
         <v>168</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D60" s="1">
@@ -3859,7 +4025,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="H60" s="9" t="s">
         <v>94</v>
       </c>
       <c r="I60">
@@ -3872,8 +4038,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3910,15 +4079,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L61">
+        <v>2</v>
+      </c>
     </row>
-    <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="1">
         <v>192</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D62" s="1">
@@ -3935,7 +4107,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="H62" s="9" t="s">
         <v>96</v>
       </c>
       <c r="I62">
@@ -3948,8 +4120,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L62">
+        <v>2</v>
+      </c>
     </row>
-    <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3986,15 +4161,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L63">
+        <v>2</v>
+      </c>
     </row>
-    <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="1">
         <v>216</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>98</v>
       </c>
       <c r="D64" s="1">
@@ -4011,7 +4189,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H64" s="10" t="s">
+      <c r="H64" s="9" t="s">
         <v>98</v>
       </c>
       <c r="I64">
@@ -4024,8 +4202,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L64">
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4062,15 +4243,18 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L65">
+        <v>3</v>
+      </c>
     </row>
-    <row r="66" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1">
         <v>240</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>100</v>
       </c>
       <c r="D66" s="1">
@@ -4087,7 +4271,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H66" s="10" t="s">
+      <c r="H66" s="9" t="s">
         <v>100</v>
       </c>
       <c r="I66">
@@ -4100,8 +4284,11 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
+      <c r="L66">
+        <v>3</v>
+      </c>
     </row>
-    <row r="67" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4138,15 +4325,18 @@
         <f t="shared" ref="K67:K109" si="6">J67/120</f>
         <v>0.1</v>
       </c>
+      <c r="L67">
+        <v>3</v>
+      </c>
     </row>
-    <row r="68" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="1">
         <v>264</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="9" t="s">
         <v>102</v>
       </c>
       <c r="D68" s="1">
@@ -4163,7 +4353,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H68" s="10" t="s">
+      <c r="H68" s="9" t="s">
         <v>102</v>
       </c>
       <c r="I68">
@@ -4176,8 +4366,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L68">
+        <v>3</v>
+      </c>
     </row>
-    <row r="69" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4214,15 +4407,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L69">
+        <v>3</v>
+      </c>
     </row>
-    <row r="70" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="1">
         <v>288</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="9" t="s">
         <v>104</v>
       </c>
       <c r="D70" s="1">
@@ -4239,7 +4435,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H70" s="10" t="s">
+      <c r="H70" s="9" t="s">
         <v>104</v>
       </c>
       <c r="I70">
@@ -4252,8 +4448,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L70">
+        <v>4</v>
+      </c>
     </row>
-    <row r="71" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4290,15 +4489,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L71">
+        <v>4</v>
+      </c>
     </row>
-    <row r="72" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" s="1">
         <v>312</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D72" s="1">
@@ -4315,7 +4517,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H72" s="10" t="s">
+      <c r="H72" s="9" t="s">
         <v>106</v>
       </c>
       <c r="I72">
@@ -4328,8 +4530,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L72">
+        <v>4</v>
+      </c>
     </row>
-    <row r="73" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4366,15 +4571,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L73">
+        <v>4</v>
+      </c>
     </row>
-    <row r="74" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" s="1">
         <v>336</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" s="9" t="s">
         <v>108</v>
       </c>
       <c r="D74" s="1">
@@ -4391,7 +4599,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H74" s="10" t="s">
+      <c r="H74" s="9" t="s">
         <v>108</v>
       </c>
       <c r="I74">
@@ -4404,8 +4612,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L74">
+        <v>4</v>
+      </c>
     </row>
-    <row r="75" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4442,15 +4653,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L75">
+        <v>5</v>
+      </c>
     </row>
-    <row r="76" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" s="1">
         <v>360</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="9" t="s">
         <v>110</v>
       </c>
       <c r="D76" s="1">
@@ -4467,7 +4681,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H76" s="10" t="s">
+      <c r="H76" s="9" t="s">
         <v>110</v>
       </c>
       <c r="I76">
@@ -4480,8 +4694,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L76">
+        <v>5</v>
+      </c>
     </row>
-    <row r="77" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4518,15 +4735,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L77">
+        <v>5</v>
+      </c>
     </row>
-    <row r="78" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="1">
         <v>384</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D78" s="1">
@@ -4543,7 +4763,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H78" s="10" t="s">
+      <c r="H78" s="9" t="s">
         <v>112</v>
       </c>
       <c r="I78">
@@ -4556,8 +4776,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L78">
+        <v>5</v>
+      </c>
     </row>
-    <row r="79" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4594,15 +4817,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L79">
+        <v>5</v>
+      </c>
     </row>
-    <row r="80" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" s="1">
         <v>408</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C80" s="9" t="s">
         <v>114</v>
       </c>
       <c r="D80" s="1">
@@ -4619,7 +4845,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H80" s="10" t="s">
+      <c r="H80" s="9" t="s">
         <v>114</v>
       </c>
       <c r="I80">
@@ -4632,8 +4858,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L80">
+        <v>6</v>
+      </c>
     </row>
-    <row r="81" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4670,15 +4899,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L81">
+        <v>6</v>
+      </c>
     </row>
-    <row r="82" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82" s="1">
         <v>432</v>
       </c>
-      <c r="C82" s="10" t="s">
+      <c r="C82" s="9" t="s">
         <v>116</v>
       </c>
       <c r="D82" s="1">
@@ -4695,7 +4927,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H82" s="10" t="s">
+      <c r="H82" s="9" t="s">
         <v>116</v>
       </c>
       <c r="I82">
@@ -4708,8 +4940,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L82">
+        <v>6</v>
+      </c>
     </row>
-    <row r="83" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4746,15 +4981,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L83">
+        <v>6</v>
+      </c>
     </row>
-    <row r="84" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="1">
         <v>456</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="9" t="s">
         <v>139</v>
       </c>
       <c r="D84" s="1">
@@ -4771,7 +5009,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H84" s="10" t="s">
+      <c r="H84" s="9" t="s">
         <v>139</v>
       </c>
       <c r="I84">
@@ -4784,8 +5022,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L84">
+        <v>6</v>
+      </c>
     </row>
-    <row r="85" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4822,15 +5063,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L85">
+        <v>7</v>
+      </c>
     </row>
-    <row r="86" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
         <v>85</v>
       </c>
       <c r="B86" s="1">
         <v>480</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C86" s="9" t="s">
         <v>118</v>
       </c>
       <c r="D86" s="1">
@@ -4847,7 +5091,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H86" s="10" t="s">
+      <c r="H86" s="9" t="s">
         <v>118</v>
       </c>
       <c r="I86">
@@ -4860,8 +5104,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L86">
+        <v>7</v>
+      </c>
     </row>
-    <row r="87" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4898,15 +5145,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L87">
+        <v>7</v>
+      </c>
     </row>
-    <row r="88" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="1">
         <v>504</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C88" s="9" t="s">
         <v>120</v>
       </c>
       <c r="D88" s="1">
@@ -4923,7 +5173,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H88" s="10" t="s">
+      <c r="H88" s="9" t="s">
         <v>120</v>
       </c>
       <c r="I88">
@@ -4936,8 +5186,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L88">
+        <v>7</v>
+      </c>
     </row>
-    <row r="89" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4974,15 +5227,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L89">
+        <v>7</v>
+      </c>
     </row>
-    <row r="90" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
         <v>89</v>
       </c>
       <c r="B90" s="1">
         <v>528</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C90" s="9" t="s">
         <v>122</v>
       </c>
       <c r="D90" s="1">
@@ -4999,7 +5255,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H90" s="10" t="s">
+      <c r="H90" s="9" t="s">
         <v>122</v>
       </c>
       <c r="I90">
@@ -5012,8 +5268,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L90">
+        <v>8</v>
+      </c>
     </row>
-    <row r="91" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5050,15 +5309,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L91">
+        <v>8</v>
+      </c>
     </row>
-    <row r="92" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
         <v>91</v>
       </c>
       <c r="B92" s="1">
         <v>552</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C92" s="9" t="s">
         <v>124</v>
       </c>
       <c r="D92" s="1">
@@ -5075,7 +5337,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H92" s="10" t="s">
+      <c r="H92" s="9" t="s">
         <v>124</v>
       </c>
       <c r="I92">
@@ -5088,8 +5350,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L92">
+        <v>8</v>
+      </c>
     </row>
-    <row r="93" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5126,15 +5391,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L93">
+        <v>8</v>
+      </c>
     </row>
-    <row r="94" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" s="1">
         <v>576</v>
       </c>
-      <c r="C94" s="10" t="s">
+      <c r="C94" s="9" t="s">
         <v>126</v>
       </c>
       <c r="D94" s="1">
@@ -5151,7 +5419,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H94" s="10" t="s">
+      <c r="H94" s="9" t="s">
         <v>126</v>
       </c>
       <c r="I94">
@@ -5164,8 +5432,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L94">
+        <v>8</v>
+      </c>
     </row>
-    <row r="95" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5202,15 +5473,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L95">
+        <v>9</v>
+      </c>
     </row>
-    <row r="96" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
         <v>95</v>
       </c>
       <c r="B96" s="1">
         <v>600</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C96" s="9" t="s">
         <v>128</v>
       </c>
       <c r="D96" s="1">
@@ -5227,7 +5501,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H96" s="10" t="s">
+      <c r="H96" s="9" t="s">
         <v>128</v>
       </c>
       <c r="I96">
@@ -5240,8 +5514,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L96">
+        <v>9</v>
+      </c>
     </row>
-    <row r="97" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -5278,15 +5555,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L97">
+        <v>9</v>
+      </c>
     </row>
-    <row r="98" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" s="1">
         <v>624</v>
       </c>
-      <c r="C98" s="10" t="s">
+      <c r="C98" s="9" t="s">
         <v>130</v>
       </c>
       <c r="D98" s="1">
@@ -5303,7 +5583,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H98" s="10" t="s">
+      <c r="H98" s="9" t="s">
         <v>130</v>
       </c>
       <c r="I98">
@@ -5316,8 +5596,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L98">
+        <v>9</v>
+      </c>
     </row>
-    <row r="99" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -5354,15 +5637,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L99">
+        <v>9</v>
+      </c>
     </row>
-    <row r="100" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" s="1">
         <v>648</v>
       </c>
-      <c r="C100" s="10" t="s">
+      <c r="C100" s="9" t="s">
         <v>132</v>
       </c>
       <c r="D100" s="1">
@@ -5379,7 +5665,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H100" s="10" t="s">
+      <c r="H100" s="9" t="s">
         <v>132</v>
       </c>
       <c r="I100">
@@ -5392,8 +5678,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L100">
+        <v>10</v>
+      </c>
     </row>
-    <row r="101" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -5430,15 +5719,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L101">
+        <v>10</v>
+      </c>
     </row>
-    <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1">
         <v>672</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="C102" s="9" t="s">
         <v>134</v>
       </c>
       <c r="D102" s="1">
@@ -5455,7 +5747,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H102" s="10" t="s">
+      <c r="H102" s="9" t="s">
         <v>134</v>
       </c>
       <c r="I102">
@@ -5468,8 +5760,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L102">
+        <v>10</v>
+      </c>
     </row>
-    <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -5506,15 +5801,18 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L103">
+        <v>10</v>
+      </c>
     </row>
-    <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" s="1">
         <v>696</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C104" s="9" t="s">
         <v>136</v>
       </c>
       <c r="D104" s="1">
@@ -5531,7 +5829,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H104" s="10" t="s">
+      <c r="H104" s="9" t="s">
         <v>136</v>
       </c>
       <c r="I104">
@@ -5544,8 +5842,11 @@
         <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
+      <c r="L104">
+        <v>10</v>
+      </c>
     </row>
-    <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -5582,15 +5883,18 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="L105">
+        <v>10</v>
+      </c>
     </row>
-    <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
         <v>105</v>
       </c>
       <c r="B106" s="1">
         <v>720</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="C106" s="9" t="s">
         <v>140</v>
       </c>
       <c r="D106" s="1">
@@ -5607,7 +5911,7 @@
         <f>1/3650</f>
         <v>2.7397260273972601E-4</v>
       </c>
-      <c r="H106" s="10" t="s">
+      <c r="H106" s="9" t="s">
         <v>140</v>
       </c>
       <c r="I106">
@@ -5620,8 +5924,11 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="L106">
+        <v>11</v>
+      </c>
     </row>
-    <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -5658,15 +5965,18 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="L107">
+        <v>11</v>
+      </c>
     </row>
-    <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
         <v>107</v>
       </c>
       <c r="B108" s="1">
         <v>960</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C108" s="9" t="s">
         <v>142</v>
       </c>
       <c r="D108" s="1">
@@ -5683,7 +5993,7 @@
         <f t="shared" si="8"/>
         <v>2.7397260273972601E-4</v>
       </c>
-      <c r="H108" s="10" t="s">
+      <c r="H108" s="9" t="s">
         <v>142</v>
       </c>
       <c r="I108">
@@ -5696,8 +6006,11 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="L108">
+        <v>11</v>
+      </c>
     </row>
-    <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -5734,22 +6047,25 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="L109">
+        <v>11</v>
+      </c>
     </row>
-    <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="10"/>
+      <c r="C110" s="9"/>
       <c r="D110" s="3"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="3"/>
-      <c r="H110" s="10"/>
+      <c r="H110" s="9"/>
       <c r="J110" s="1"/>
     </row>
-    <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B112" s="1"/>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5831,7 +6147,7 @@
       <c r="B138" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5840,7 +6156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0439F58-195A-FC4B-BFD4-9EADB89FDAA6}">
   <dimension ref="A1:AF110"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
@@ -6184,187 +6500,187 @@
       <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A50" s="10"/>
+      <c r="A50" s="9"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A52" s="10"/>
+      <c r="A52" s="9"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A54" s="10"/>
+      <c r="A54" s="9"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A56" s="10"/>
+      <c r="A56" s="9"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A58" s="10"/>
+      <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A60" s="10"/>
+      <c r="A60" s="9"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A62" s="10"/>
+      <c r="A62" s="9"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A64" s="10"/>
+      <c r="A64" s="9"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" s="1"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A66" s="10"/>
+      <c r="A66" s="9"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" s="1"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A68" s="10"/>
+      <c r="A68" s="9"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A70" s="10"/>
+      <c r="A70" s="9"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" s="1"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A72" s="10"/>
+      <c r="A72" s="9"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" s="1"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A74" s="10"/>
+      <c r="A74" s="9"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" s="1"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A76" s="10"/>
+      <c r="A76" s="9"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A77" s="1"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A78" s="10"/>
+      <c r="A78" s="9"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A79" s="1"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A80" s="10"/>
+      <c r="A80" s="9"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A82" s="10"/>
+      <c r="A82" s="9"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A83" s="1"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A84" s="10"/>
+      <c r="A84" s="9"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A85" s="1"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A86" s="10"/>
+      <c r="A86" s="9"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A87" s="1"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A88" s="10"/>
+      <c r="A88" s="9"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A89" s="1"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A90" s="10"/>
+      <c r="A90" s="9"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" s="1"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A92" s="10"/>
+      <c r="A92" s="9"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" s="1"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A94" s="10"/>
+      <c r="A94" s="9"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A95" s="1"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A96" s="10"/>
+      <c r="A96" s="9"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" s="1"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A98" s="10"/>
+      <c r="A98" s="9"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A99" s="1"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A100" s="10"/>
+      <c r="A100" s="9"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A101" s="1"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A102" s="10"/>
+      <c r="A102" s="9"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A103" s="1"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A104" s="10"/>
+      <c r="A104" s="9"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A105" s="1"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A106" s="10"/>
+      <c r="A106" s="9"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A107" s="1"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A108" s="10"/>
+      <c r="A108" s="9"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A109" s="1"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A110" s="10"/>
+      <c r="A110" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11184,7 +11500,7 @@
       </c>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B50">
@@ -11380,7 +11696,7 @@
       </c>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="9" t="s">
         <v>86</v>
       </c>
       <c r="B52">
@@ -11576,7 +11892,7 @@
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="9" t="s">
         <v>88</v>
       </c>
       <c r="B54">
@@ -11772,7 +12088,7 @@
       </c>
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B56">
@@ -11968,7 +12284,7 @@
       </c>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B58">
@@ -12164,7 +12480,7 @@
       </c>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B60">
@@ -12360,7 +12676,7 @@
       </c>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B62">
@@ -12556,7 +12872,7 @@
       </c>
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B64">
@@ -12752,7 +13068,7 @@
       </c>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B66">
@@ -12948,7 +13264,7 @@
       </c>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B68">
@@ -13144,7 +13460,7 @@
       </c>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B70">
@@ -13340,7 +13656,7 @@
       </c>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B72">
@@ -13536,7 +13852,7 @@
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B74">
@@ -13732,7 +14048,7 @@
       </c>
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B76">
@@ -13928,7 +14244,7 @@
       </c>
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B78">
@@ -14124,7 +14440,7 @@
       </c>
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B80">
@@ -14320,7 +14636,7 @@
       </c>
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B82">
@@ -14516,7 +14832,7 @@
       </c>
     </row>
     <row r="84" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A84" s="10" t="s">
+      <c r="A84" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B84">
@@ -14712,7 +15028,7 @@
       </c>
     </row>
     <row r="86" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B86">
@@ -14908,7 +15224,7 @@
       </c>
     </row>
     <row r="88" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A88" s="10" t="s">
+      <c r="A88" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B88">
@@ -15104,7 +15420,7 @@
       </c>
     </row>
     <row r="90" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="9" t="s">
         <v>122</v>
       </c>
       <c r="B90">
@@ -15300,7 +15616,7 @@
       </c>
     </row>
     <row r="92" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="9" t="s">
         <v>124</v>
       </c>
       <c r="B92">
@@ -15496,7 +15812,7 @@
       </c>
     </row>
     <row r="94" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A94" s="10" t="s">
+      <c r="A94" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B94">
@@ -15692,7 +16008,7 @@
       </c>
     </row>
     <row r="96" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B96">
@@ -15888,7 +16204,7 @@
       </c>
     </row>
     <row r="98" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="9" t="s">
         <v>130</v>
       </c>
       <c r="B98">
@@ -16084,7 +16400,7 @@
       </c>
     </row>
     <row r="100" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A100" s="10" t="s">
+      <c r="A100" s="9" t="s">
         <v>132</v>
       </c>
       <c r="B100">
@@ -16280,7 +16596,7 @@
       </c>
     </row>
     <row r="102" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="9" t="s">
         <v>134</v>
       </c>
       <c r="B102">
@@ -16476,7 +16792,7 @@
       </c>
     </row>
     <row r="104" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A104" s="10" t="s">
+      <c r="A104" s="9" t="s">
         <v>136</v>
       </c>
       <c r="B104">
@@ -16672,7 +16988,7 @@
       </c>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A106" s="10" t="s">
+      <c r="A106" s="9" t="s">
         <v>160</v>
       </c>
       <c r="B106">
@@ -16868,7 +17184,7 @@
       </c>
     </row>
     <row r="108" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A108" s="10" t="s">
+      <c r="A108" s="9" t="s">
         <v>162</v>
       </c>
       <c r="B108">
@@ -17064,7 +17380,7 @@
       </c>
     </row>
     <row r="110" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A110" s="10"/>
+      <c r="A110" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AF110">
@@ -17112,13 +17428,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -17189,7 +17505,7 @@
   </sheetPr>
   <dimension ref="A1:DF119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB13" zoomScale="42" workbookViewId="0">
+    <sheetView topLeftCell="BB13" zoomScale="42" workbookViewId="0">
       <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
@@ -17346,187 +17662,187 @@
       <c r="AW1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AX1" s="10" t="s">
+      <c r="AX1" s="9" t="s">
         <v>84</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AZ1" s="10" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>86</v>
       </c>
       <c r="BA1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BB1" s="10" t="s">
+      <c r="BB1" s="9" t="s">
         <v>88</v>
       </c>
       <c r="BC1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="BD1" s="10" t="s">
+      <c r="BD1" s="9" t="s">
         <v>90</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BF1" s="10" t="s">
+      <c r="BF1" s="9" t="s">
         <v>92</v>
       </c>
       <c r="BG1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="BH1" s="10" t="s">
+      <c r="BH1" s="9" t="s">
         <v>94</v>
       </c>
       <c r="BI1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BJ1" s="10" t="s">
+      <c r="BJ1" s="9" t="s">
         <v>96</v>
       </c>
       <c r="BK1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="BL1" s="10" t="s">
+      <c r="BL1" s="9" t="s">
         <v>98</v>
       </c>
       <c r="BM1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="BN1" s="10" t="s">
+      <c r="BN1" s="9" t="s">
         <v>100</v>
       </c>
       <c r="BO1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="BP1" s="10" t="s">
+      <c r="BP1" s="9" t="s">
         <v>102</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BR1" s="10" t="s">
+      <c r="BR1" s="9" t="s">
         <v>104</v>
       </c>
       <c r="BS1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="BT1" s="10" t="s">
+      <c r="BT1" s="9" t="s">
         <v>106</v>
       </c>
       <c r="BU1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BV1" s="10" t="s">
+      <c r="BV1" s="9" t="s">
         <v>108</v>
       </c>
       <c r="BW1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BX1" s="10" t="s">
+      <c r="BX1" s="9" t="s">
         <v>110</v>
       </c>
       <c r="BY1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BZ1" s="10" t="s">
+      <c r="BZ1" s="9" t="s">
         <v>112</v>
       </c>
       <c r="CA1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="CB1" s="10" t="s">
+      <c r="CB1" s="9" t="s">
         <v>114</v>
       </c>
       <c r="CC1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="CD1" s="10" t="s">
+      <c r="CD1" s="9" t="s">
         <v>116</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="CF1" s="10" t="s">
+      <c r="CF1" s="9" t="s">
         <v>139</v>
       </c>
       <c r="CG1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="CH1" s="10" t="s">
+      <c r="CH1" s="9" t="s">
         <v>118</v>
       </c>
       <c r="CI1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="CJ1" s="10" t="s">
+      <c r="CJ1" s="9" t="s">
         <v>120</v>
       </c>
       <c r="CK1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="CL1" s="10" t="s">
+      <c r="CL1" s="9" t="s">
         <v>122</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="CN1" s="10" t="s">
+      <c r="CN1" s="9" t="s">
         <v>124</v>
       </c>
       <c r="CO1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="CP1" s="10" t="s">
+      <c r="CP1" s="9" t="s">
         <v>126</v>
       </c>
       <c r="CQ1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="CR1" s="10" t="s">
+      <c r="CR1" s="9" t="s">
         <v>128</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="CT1" s="10" t="s">
+      <c r="CT1" s="9" t="s">
         <v>130</v>
       </c>
       <c r="CU1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="CV1" s="10" t="s">
+      <c r="CV1" s="9" t="s">
         <v>132</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="CX1" s="10" t="s">
+      <c r="CX1" s="9" t="s">
         <v>134</v>
       </c>
       <c r="CY1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="CZ1" s="10" t="s">
+      <c r="CZ1" s="9" t="s">
         <v>136</v>
       </c>
       <c r="DA1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="DB1" s="10" t="s">
+      <c r="DB1" s="9" t="s">
         <v>140</v>
       </c>
       <c r="DC1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="DD1" s="10" t="s">
+      <c r="DD1" s="9" t="s">
         <v>142</v>
       </c>
       <c r="DE1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="DF1" s="10"/>
+      <c r="DF1" s="9"/>
     </row>
     <row r="2" spans="1:110" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -33321,7 +33637,7 @@
       </c>
     </row>
     <row r="50" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B50">
@@ -33979,7 +34295,7 @@
       </c>
     </row>
     <row r="52" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="9" t="s">
         <v>86</v>
       </c>
       <c r="B52">
@@ -34637,7 +34953,7 @@
       </c>
     </row>
     <row r="54" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="9" t="s">
         <v>88</v>
       </c>
       <c r="B54">
@@ -35295,7 +35611,7 @@
       </c>
     </row>
     <row r="56" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B56">
@@ -35953,7 +36269,7 @@
       </c>
     </row>
     <row r="58" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B58">
@@ -36611,7 +36927,7 @@
       </c>
     </row>
     <row r="60" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B60">
@@ -37269,7 +37585,7 @@
       </c>
     </row>
     <row r="62" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B62">
@@ -37927,7 +38243,7 @@
       </c>
     </row>
     <row r="64" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B64">
@@ -38585,7 +38901,7 @@
       </c>
     </row>
     <row r="66" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B66">
@@ -39243,7 +39559,7 @@
       </c>
     </row>
     <row r="68" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B68">
@@ -39901,7 +40217,7 @@
       </c>
     </row>
     <row r="70" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B70">
@@ -40559,7 +40875,7 @@
       </c>
     </row>
     <row r="72" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B72">
@@ -41217,7 +41533,7 @@
       </c>
     </row>
     <row r="74" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B74">
@@ -41875,7 +42191,7 @@
       </c>
     </row>
     <row r="76" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B76">
@@ -42533,7 +42849,7 @@
       </c>
     </row>
     <row r="78" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B78">
@@ -43191,7 +43507,7 @@
       </c>
     </row>
     <row r="80" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B80">
@@ -43849,7 +44165,7 @@
       </c>
     </row>
     <row r="82" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B82">
@@ -44507,7 +44823,7 @@
       </c>
     </row>
     <row r="84" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="10" t="s">
+      <c r="A84" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B84">
@@ -45165,7 +45481,7 @@
       </c>
     </row>
     <row r="86" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B86">
@@ -45823,7 +46139,7 @@
       </c>
     </row>
     <row r="88" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="10" t="s">
+      <c r="A88" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B88">
@@ -46481,7 +46797,7 @@
       </c>
     </row>
     <row r="90" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="9" t="s">
         <v>122</v>
       </c>
       <c r="B90">
@@ -47139,7 +47455,7 @@
       </c>
     </row>
     <row r="92" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="9" t="s">
         <v>124</v>
       </c>
       <c r="B92">
@@ -47797,7 +48113,7 @@
       </c>
     </row>
     <row r="94" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="10" t="s">
+      <c r="A94" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B94">
@@ -48455,7 +48771,7 @@
       </c>
     </row>
     <row r="96" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B96">
@@ -49113,7 +49429,7 @@
       </c>
     </row>
     <row r="98" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="9" t="s">
         <v>130</v>
       </c>
       <c r="B98">
@@ -49771,7 +50087,7 @@
       </c>
     </row>
     <row r="100" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="10" t="s">
+      <c r="A100" s="9" t="s">
         <v>132</v>
       </c>
       <c r="B100">
@@ -50429,7 +50745,7 @@
       </c>
     </row>
     <row r="102" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="9" t="s">
         <v>134</v>
       </c>
       <c r="B102">
@@ -51087,7 +51403,7 @@
       </c>
     </row>
     <row r="104" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="10" t="s">
+      <c r="A104" s="9" t="s">
         <v>136</v>
       </c>
       <c r="B104">
@@ -51745,7 +52061,7 @@
       </c>
     </row>
     <row r="106" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="10" t="s">
+      <c r="A106" s="9" t="s">
         <v>140</v>
       </c>
       <c r="B106">
@@ -52403,7 +52719,7 @@
       </c>
     </row>
     <row r="108" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="10" t="s">
+      <c r="A108" s="9" t="s">
         <v>142</v>
       </c>
       <c r="B108">
@@ -53061,10 +53377,10 @@
       </c>
     </row>
     <row r="110" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="10"/>
+      <c r="A110" s="9"/>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B113" s="6" t="s">
+      <c r="B113" s="5" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>